<commit_message>
Dell XPS' Update Signed off by: Luca Inghilterra E-mail: 271539@studenti.unimore.it
</commit_message>
<xml_diff>
--- a/src/mcat/Grid Search.xlsx
+++ b/src/mcat/Grid Search.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucai\Desktop\Magistrale\Tirocinio\AIforBioinformatics\src\mcat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600102B7-DE4C-4E0F-B650-1AD3823E3DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB9F596-7CC9-4F70-B119-66224AF8A1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="77">
   <si>
     <t>Alpha</t>
   </si>
@@ -156,9 +156,6 @@
     <t>lucas_job 2506978</t>
   </si>
   <si>
-    <t>lucas_job 2506979</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Mean: 0.5983, Variance: 0.0007, 95% Confidence Interval: [0.5757, 0.6209]</t>
   </si>
   <si>
@@ -193,6 +190,72 @@
   </si>
   <si>
     <t>[1.3337, 1.2914, 1.4191, 1.3301, 1.2975]</t>
+  </si>
+  <si>
+    <t>0.925</t>
+  </si>
+  <si>
+    <t>0.875</t>
+  </si>
+  <si>
+    <t>lucas_job 2506982</t>
+  </si>
+  <si>
+    <t>lucas_job 2506983</t>
+  </si>
+  <si>
+    <t>lucas_job 2506984</t>
+  </si>
+  <si>
+    <t>lucas_job 2506985</t>
+  </si>
+  <si>
+    <t>Mean: 0.6131, Variance: 0.0013, 95% Confidence Interval: [0.5815, 0.6446]</t>
+  </si>
+  <si>
+    <t>[1.7374, 1.5952, 1.6373, 0.9172, 1.1172]</t>
+  </si>
+  <si>
+    <t>Mean: 1.4008, Variance: 0.1303, 95% Confidence Interval: [1.0844, 1.7173]</t>
+  </si>
+  <si>
+    <t>[0.6192, 0.5914, 0.5863, 0.6734, 0.5952]</t>
+  </si>
+  <si>
+    <t>Mean: 0.6116, Variance: 0.0022, 95% Confidence Interval: [0.5707, 0.6524]</t>
+  </si>
+  <si>
+    <t>Mean: 1.5437, Variance: 0.0804, 95% Confidence Interval: [1.2951, 1.7923]</t>
+  </si>
+  <si>
+    <t>[0.6411, 0.5657, 0.5755, 0.6767, 0.5989]</t>
+  </si>
+  <si>
+    <t>[1.8036, 1.7127, 1.7294, 1.2695, 1.2032]</t>
+  </si>
+  <si>
+    <t>Mean: 0.6105, Variance: 0.0027, 95% Confidence Interval: [0.5649, 0.6560]</t>
+  </si>
+  <si>
+    <t>Mean: 1.6077, Variance: 0.0676, 95% Confidence Interval: [1.3798, 1.8355]</t>
+  </si>
+  <si>
+    <t>[0.6432, 0.5536, 0.5708, 0.6805, 0.6043]</t>
+  </si>
+  <si>
+    <t>[1.8414, 1.7697, 1.7774, 1.3440, 1.3058]</t>
+  </si>
+  <si>
+    <t>Mean: 0.6110, Variance: 0.0017, 95% Confidence Interval: [0.5747, 0.6474]</t>
+  </si>
+  <si>
+    <t>[0.6288, 0.5782, 0.5764, 0.6750, 0.5968]</t>
+  </si>
+  <si>
+    <t>Mean: 1.4794, Variance: 0.0976, 95% Confidence Interval: [1.2055, 1.7532]</t>
+  </si>
+  <si>
+    <t>[1.7683, 1.6620, 1.6821, 1.1931, 1.0913]</t>
   </si>
 </sst>
 </file>
@@ -227,7 +290,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,6 +312,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -306,6 +375,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -594,37 +669,37 @@
   <dimension ref="A1:V49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z14" sqref="Z14"/>
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.26953125" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" customWidth="1"/>
-    <col min="4" max="4" width="10.90625" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" customWidth="1"/>
-    <col min="7" max="7" width="24.08984375" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="40.21875" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" customWidth="1"/>
+    <col min="7" max="7" width="24.109375" customWidth="1"/>
+    <col min="9" max="9" width="26.21875" customWidth="1"/>
     <col min="11" max="11" width="7" customWidth="1"/>
-    <col min="12" max="12" width="14.81640625" customWidth="1"/>
-    <col min="13" max="13" width="9.453125" customWidth="1"/>
-    <col min="14" max="14" width="10.453125" customWidth="1"/>
-    <col min="15" max="15" width="10.26953125" customWidth="1"/>
-    <col min="16" max="16" width="13.90625" customWidth="1"/>
-    <col min="17" max="17" width="15.26953125" customWidth="1"/>
-    <col min="18" max="18" width="13.54296875" customWidth="1"/>
-    <col min="19" max="19" width="65.1796875" customWidth="1"/>
-    <col min="20" max="20" width="37.08984375" customWidth="1"/>
-    <col min="21" max="21" width="64.453125" customWidth="1"/>
-    <col min="22" max="22" width="38.6328125" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" customWidth="1"/>
+    <col min="15" max="15" width="10.21875" customWidth="1"/>
+    <col min="16" max="16" width="13.88671875" customWidth="1"/>
+    <col min="17" max="17" width="15.21875" customWidth="1"/>
+    <col min="18" max="18" width="13.5546875" customWidth="1"/>
+    <col min="19" max="19" width="65.21875" customWidth="1"/>
+    <col min="20" max="20" width="37.109375" customWidth="1"/>
+    <col min="21" max="21" width="64.44140625" customWidth="1"/>
+    <col min="22" max="22" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -689,7 +764,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
@@ -699,16 +774,16 @@
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="7">
         <v>1</v>
       </c>
       <c r="E3" s="3">
         <v>20</v>
       </c>
-      <c r="F3" s="3">
-        <v>100</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="F3" s="7">
+        <v>100</v>
+      </c>
+      <c r="G3" s="7">
         <v>7</v>
       </c>
       <c r="H3" s="3" t="s">
@@ -720,28 +795,28 @@
       <c r="J3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="3" t="s">
+      <c r="M3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" s="3" t="s">
+      <c r="Q3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S3" s="3" t="s">
@@ -757,7 +832,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
@@ -767,16 +842,16 @@
       <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="7">
         <v>1</v>
       </c>
       <c r="E4" s="3">
         <v>20</v>
       </c>
-      <c r="F4" s="3">
-        <v>100</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="F4" s="7">
+        <v>100</v>
+      </c>
+      <c r="G4" s="7">
         <v>7</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -788,44 +863,44 @@
       <c r="J4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="3" t="s">
+      <c r="M4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" s="3" t="s">
+      <c r="Q4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -835,16 +910,16 @@
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="7">
         <v>1</v>
       </c>
       <c r="E5" s="3">
         <v>20</v>
       </c>
-      <c r="F5" s="3">
-        <v>100</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="F5" s="7">
+        <v>100</v>
+      </c>
+      <c r="G5" s="7">
         <v>7</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -856,40 +931,44 @@
       <c r="J5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R5" s="3" t="s">
+      <c r="K5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="U5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="T5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="V5" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
@@ -899,16 +978,16 @@
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="7">
         <v>1</v>
       </c>
       <c r="E6" s="3">
         <v>20</v>
       </c>
-      <c r="F6" s="3">
-        <v>100</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="F6" s="7">
+        <v>100</v>
+      </c>
+      <c r="G6" s="7">
         <v>7</v>
       </c>
       <c r="H6" s="3" t="s">
@@ -920,42 +999,46 @@
       <c r="J6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R6" s="3" t="s">
+      <c r="K6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R6" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="U6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="T6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="V6" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>3</v>
@@ -963,16 +1046,16 @@
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="7">
         <v>1</v>
       </c>
       <c r="E7" s="3">
         <v>20</v>
       </c>
-      <c r="F7" s="3">
-        <v>100</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="F7" s="7">
+        <v>100</v>
+      </c>
+      <c r="G7" s="7">
         <v>7</v>
       </c>
       <c r="H7" s="3" t="s">
@@ -984,204 +1067,284 @@
       <c r="J7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3">
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="7">
         <v>1</v>
       </c>
       <c r="E8" s="3">
         <v>20</v>
       </c>
-      <c r="F8" s="3">
-        <v>100</v>
-      </c>
-      <c r="G8" s="3">
-        <v>7</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="F8" s="7">
+        <v>100</v>
+      </c>
+      <c r="G8" s="7">
+        <v>7</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="3">
+        <v>4</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="T8" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3">
+      <c r="C9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="7">
         <v>1</v>
       </c>
       <c r="E9" s="3">
         <v>20</v>
       </c>
-      <c r="F9" s="3">
-        <v>100</v>
-      </c>
-      <c r="G9" s="3">
-        <v>7</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="F9" s="7">
+        <v>100</v>
+      </c>
+      <c r="G9" s="7">
+        <v>7</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="3">
+        <v>4</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3">
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="7">
         <v>1</v>
       </c>
       <c r="E10" s="3">
         <v>20</v>
       </c>
-      <c r="F10" s="3">
-        <v>100</v>
-      </c>
-      <c r="G10" s="3">
-        <v>7</v>
-      </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="F10" s="7">
+        <v>100</v>
+      </c>
+      <c r="G10" s="7">
+        <v>7</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="3">
+        <v>4</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="3">
+      <c r="D11" s="7">
         <v>1</v>
       </c>
       <c r="E11" s="3">
         <v>20</v>
       </c>
-      <c r="F11" s="3">
-        <v>100</v>
-      </c>
-      <c r="G11" s="3">
-        <v>7</v>
-      </c>
-      <c r="H11" s="3"/>
+      <c r="F11" s="7">
+        <v>100</v>
+      </c>
+      <c r="G11" s="7">
+        <v>7</v>
+      </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="3" t="s">
+      <c r="K11" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L11" s="3"/>
-      <c r="M11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O11" s="3" t="s">
+      <c r="M11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P11" s="3"/>
-      <c r="Q11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R11" s="3" t="s">
+      <c r="Q11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R11" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S11" s="3"/>
@@ -1189,44 +1352,44 @@
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="3">
+      <c r="D12" s="7">
         <v>1</v>
       </c>
       <c r="E12" s="3">
         <v>20</v>
       </c>
-      <c r="F12" s="3">
-        <v>100</v>
-      </c>
-      <c r="G12" s="3">
+      <c r="F12" s="7">
+        <v>100</v>
+      </c>
+      <c r="G12" s="7">
         <v>7</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L12" s="3"/>
-      <c r="M12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O12" s="3" t="s">
+      <c r="M12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P12" s="3"/>
-      <c r="Q12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R12" s="3" t="s">
+      <c r="Q12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R12" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S12" s="3"/>
@@ -1234,44 +1397,44 @@
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="3">
+      <c r="D13" s="7">
         <v>1</v>
       </c>
       <c r="E13" s="3">
         <v>20</v>
       </c>
-      <c r="F13" s="3">
-        <v>100</v>
-      </c>
-      <c r="G13" s="3">
+      <c r="F13" s="7">
+        <v>100</v>
+      </c>
+      <c r="G13" s="7">
         <v>7</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L13" s="3"/>
-      <c r="M13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O13" s="3" t="s">
+      <c r="M13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P13" s="3"/>
-      <c r="Q13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R13" s="3" t="s">
+      <c r="Q13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R13" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S13" s="3"/>
@@ -1279,44 +1442,44 @@
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="3">
+      <c r="D14" s="7">
         <v>1</v>
       </c>
       <c r="E14" s="3">
         <v>20</v>
       </c>
-      <c r="F14" s="3">
-        <v>100</v>
-      </c>
-      <c r="G14" s="3">
+      <c r="F14" s="7">
+        <v>100</v>
+      </c>
+      <c r="G14" s="7">
         <v>7</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-      <c r="K14" s="3" t="s">
+      <c r="K14" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L14" s="3"/>
-      <c r="M14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O14" s="3" t="s">
+      <c r="M14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O14" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P14" s="3"/>
-      <c r="Q14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R14" s="3" t="s">
+      <c r="Q14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R14" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S14" s="3"/>
@@ -1324,44 +1487,44 @@
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="3">
+      <c r="D15" s="7">
         <v>1</v>
       </c>
       <c r="E15" s="3">
         <v>20</v>
       </c>
-      <c r="F15" s="3">
-        <v>100</v>
-      </c>
-      <c r="G15" s="3">
+      <c r="F15" s="7">
+        <v>100</v>
+      </c>
+      <c r="G15" s="7">
         <v>7</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
-      <c r="K15" s="3" t="s">
+      <c r="K15" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L15" s="3"/>
-      <c r="M15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O15" s="3" t="s">
+      <c r="M15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P15" s="3"/>
-      <c r="Q15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R15" s="3" t="s">
+      <c r="Q15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R15" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S15" s="3"/>
@@ -1369,44 +1532,44 @@
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="3">
+      <c r="D16" s="7">
         <v>1</v>
       </c>
       <c r="E16" s="3">
         <v>20</v>
       </c>
-      <c r="F16" s="3">
-        <v>100</v>
-      </c>
-      <c r="G16" s="3">
+      <c r="F16" s="7">
+        <v>100</v>
+      </c>
+      <c r="G16" s="7">
         <v>7</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="3" t="s">
+      <c r="K16" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L16" s="3"/>
-      <c r="M16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O16" s="3" t="s">
+      <c r="M16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O16" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P16" s="3"/>
-      <c r="Q16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R16" s="3" t="s">
+      <c r="Q16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R16" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S16" s="3"/>
@@ -1414,44 +1577,44 @@
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="3">
+      <c r="D17" s="7">
         <v>1</v>
       </c>
       <c r="E17" s="3">
         <v>20</v>
       </c>
-      <c r="F17" s="3">
-        <v>100</v>
-      </c>
-      <c r="G17" s="3">
+      <c r="F17" s="7">
+        <v>100</v>
+      </c>
+      <c r="G17" s="7">
         <v>7</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="3" t="s">
+      <c r="K17" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L17" s="3"/>
-      <c r="M17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O17" s="3" t="s">
+      <c r="M17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O17" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P17" s="3"/>
-      <c r="Q17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R17" s="3" t="s">
+      <c r="Q17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R17" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S17" s="3"/>
@@ -1459,44 +1622,44 @@
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="3">
+      <c r="D18" s="7">
         <v>1</v>
       </c>
       <c r="E18" s="3">
         <v>20</v>
       </c>
-      <c r="F18" s="3">
-        <v>100</v>
-      </c>
-      <c r="G18" s="3">
+      <c r="F18" s="7">
+        <v>100</v>
+      </c>
+      <c r="G18" s="7">
         <v>7</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="3" t="s">
+      <c r="K18" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L18" s="3"/>
-      <c r="M18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O18" s="3" t="s">
+      <c r="M18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O18" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P18" s="3"/>
-      <c r="Q18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R18" s="3" t="s">
+      <c r="Q18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R18" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S18" s="3"/>
@@ -1504,44 +1667,44 @@
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="3">
+      <c r="D19" s="7">
         <v>1</v>
       </c>
       <c r="E19" s="3">
         <v>20</v>
       </c>
-      <c r="F19" s="3">
-        <v>100</v>
-      </c>
-      <c r="G19" s="3">
+      <c r="F19" s="7">
+        <v>100</v>
+      </c>
+      <c r="G19" s="7">
         <v>7</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="3" t="s">
+      <c r="K19" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L19" s="3"/>
-      <c r="M19" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O19" s="3" t="s">
+      <c r="M19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O19" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P19" s="3"/>
-      <c r="Q19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R19" s="3" t="s">
+      <c r="Q19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R19" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S19" s="3"/>
@@ -1549,44 +1712,44 @@
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="3">
+      <c r="D20" s="7">
         <v>1</v>
       </c>
       <c r="E20" s="3">
         <v>20</v>
       </c>
-      <c r="F20" s="3">
-        <v>100</v>
-      </c>
-      <c r="G20" s="3">
+      <c r="F20" s="7">
+        <v>100</v>
+      </c>
+      <c r="G20" s="7">
         <v>7</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="3" t="s">
+      <c r="K20" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L20" s="3"/>
-      <c r="M20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O20" s="3" t="s">
+      <c r="M20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O20" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P20" s="3"/>
-      <c r="Q20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R20" s="3" t="s">
+      <c r="Q20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R20" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S20" s="3"/>
@@ -1594,44 +1757,44 @@
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="3">
+      <c r="D21" s="7">
         <v>1</v>
       </c>
       <c r="E21" s="3">
         <v>20</v>
       </c>
-      <c r="F21" s="3">
-        <v>100</v>
-      </c>
-      <c r="G21" s="3">
+      <c r="F21" s="7">
+        <v>100</v>
+      </c>
+      <c r="G21" s="7">
         <v>7</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
-      <c r="K21" s="3" t="s">
+      <c r="K21" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L21" s="3"/>
-      <c r="M21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O21" s="3" t="s">
+      <c r="M21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O21" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P21" s="3"/>
-      <c r="Q21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R21" s="3" t="s">
+      <c r="Q21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R21" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S21" s="3"/>
@@ -1639,44 +1802,44 @@
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
     </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="3">
+      <c r="D22" s="7">
         <v>1</v>
       </c>
       <c r="E22" s="3">
         <v>20</v>
       </c>
-      <c r="F22" s="3">
-        <v>100</v>
-      </c>
-      <c r="G22" s="3">
+      <c r="F22" s="7">
+        <v>100</v>
+      </c>
+      <c r="G22" s="7">
         <v>7</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="3" t="s">
+      <c r="K22" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L22" s="3"/>
-      <c r="M22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O22" s="3" t="s">
+      <c r="M22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O22" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P22" s="3"/>
-      <c r="Q22" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R22" s="3" t="s">
+      <c r="Q22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R22" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S22" s="3"/>
@@ -1684,44 +1847,44 @@
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
     </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="3">
+      <c r="D23" s="7">
         <v>1</v>
       </c>
       <c r="E23" s="3">
         <v>20</v>
       </c>
-      <c r="F23" s="3">
-        <v>100</v>
-      </c>
-      <c r="G23" s="3">
+      <c r="F23" s="7">
+        <v>100</v>
+      </c>
+      <c r="G23" s="7">
         <v>7</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="3" t="s">
+      <c r="K23" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L23" s="3"/>
-      <c r="M23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O23" s="3" t="s">
+      <c r="M23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O23" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P23" s="3"/>
-      <c r="Q23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R23" s="3" t="s">
+      <c r="Q23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R23" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S23" s="3"/>
@@ -1729,44 +1892,44 @@
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
     </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="3">
+      <c r="D24" s="7">
         <v>1</v>
       </c>
       <c r="E24" s="3">
         <v>20</v>
       </c>
-      <c r="F24" s="3">
-        <v>100</v>
-      </c>
-      <c r="G24" s="3">
+      <c r="F24" s="7">
+        <v>100</v>
+      </c>
+      <c r="G24" s="7">
         <v>7</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
-      <c r="K24" s="3" t="s">
+      <c r="K24" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L24" s="3"/>
-      <c r="M24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O24" s="3" t="s">
+      <c r="M24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O24" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P24" s="3"/>
-      <c r="Q24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R24" s="3" t="s">
+      <c r="Q24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R24" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S24" s="3"/>
@@ -1774,44 +1937,44 @@
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="3">
+      <c r="D25" s="7">
         <v>1</v>
       </c>
       <c r="E25" s="3">
         <v>20</v>
       </c>
-      <c r="F25" s="3">
-        <v>100</v>
-      </c>
-      <c r="G25" s="3">
+      <c r="F25" s="7">
+        <v>100</v>
+      </c>
+      <c r="G25" s="7">
         <v>7</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-      <c r="K25" s="3" t="s">
+      <c r="K25" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L25" s="3"/>
-      <c r="M25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O25" s="3" t="s">
+      <c r="M25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O25" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P25" s="3"/>
-      <c r="Q25" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R25" s="3" t="s">
+      <c r="Q25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R25" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S25" s="3"/>
@@ -1819,44 +1982,44 @@
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="3"/>
-      <c r="D26" s="3">
+      <c r="D26" s="7">
         <v>1</v>
       </c>
       <c r="E26" s="3">
         <v>20</v>
       </c>
-      <c r="F26" s="3">
-        <v>100</v>
-      </c>
-      <c r="G26" s="3">
+      <c r="F26" s="7">
+        <v>100</v>
+      </c>
+      <c r="G26" s="7">
         <v>7</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
-      <c r="K26" s="3" t="s">
+      <c r="K26" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L26" s="3"/>
-      <c r="M26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O26" s="3" t="s">
+      <c r="M26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O26" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P26" s="3"/>
-      <c r="Q26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R26" s="3" t="s">
+      <c r="Q26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R26" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S26" s="3"/>
@@ -1864,44 +2027,44 @@
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="3">
+      <c r="D27" s="7">
         <v>1</v>
       </c>
       <c r="E27" s="3">
         <v>20</v>
       </c>
-      <c r="F27" s="3">
-        <v>100</v>
-      </c>
-      <c r="G27" s="3">
+      <c r="F27" s="7">
+        <v>100</v>
+      </c>
+      <c r="G27" s="7">
         <v>7</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
-      <c r="K27" s="3" t="s">
+      <c r="K27" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L27" s="3"/>
-      <c r="M27" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O27" s="3" t="s">
+      <c r="M27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O27" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P27" s="3"/>
-      <c r="Q27" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R27" s="3" t="s">
+      <c r="Q27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R27" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S27" s="3"/>
@@ -1909,44 +2072,44 @@
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B28" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="3">
+      <c r="D28" s="7">
         <v>1</v>
       </c>
       <c r="E28" s="3">
         <v>20</v>
       </c>
-      <c r="F28" s="3">
-        <v>100</v>
-      </c>
-      <c r="G28" s="3">
+      <c r="F28" s="7">
+        <v>100</v>
+      </c>
+      <c r="G28" s="7">
         <v>7</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
-      <c r="K28" s="3" t="s">
+      <c r="K28" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L28" s="3"/>
-      <c r="M28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N28" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O28" s="3" t="s">
+      <c r="M28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O28" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P28" s="3"/>
-      <c r="Q28" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R28" s="3" t="s">
+      <c r="Q28" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R28" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S28" s="3"/>
@@ -1954,44 +2117,44 @@
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="3">
+      <c r="D29" s="7">
         <v>1</v>
       </c>
       <c r="E29" s="3">
         <v>20</v>
       </c>
-      <c r="F29" s="3">
-        <v>100</v>
-      </c>
-      <c r="G29" s="3">
+      <c r="F29" s="7">
+        <v>100</v>
+      </c>
+      <c r="G29" s="7">
         <v>7</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
-      <c r="K29" s="3" t="s">
+      <c r="K29" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L29" s="3"/>
-      <c r="M29" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O29" s="3" t="s">
+      <c r="M29" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O29" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P29" s="3"/>
-      <c r="Q29" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R29" s="3" t="s">
+      <c r="Q29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R29" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S29" s="3"/>
@@ -1999,44 +2162,44 @@
       <c r="U29" s="3"/>
       <c r="V29" s="3"/>
     </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="3"/>
-      <c r="D30" s="3">
+      <c r="D30" s="7">
         <v>1</v>
       </c>
       <c r="E30" s="3">
         <v>20</v>
       </c>
-      <c r="F30" s="3">
-        <v>100</v>
-      </c>
-      <c r="G30" s="3">
+      <c r="F30" s="7">
+        <v>100</v>
+      </c>
+      <c r="G30" s="7">
         <v>7</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="3" t="s">
+      <c r="K30" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L30" s="3"/>
-      <c r="M30" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O30" s="3" t="s">
+      <c r="M30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O30" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P30" s="3"/>
-      <c r="Q30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R30" s="3" t="s">
+      <c r="Q30" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R30" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S30" s="3"/>
@@ -2044,44 +2207,44 @@
       <c r="U30" s="3"/>
       <c r="V30" s="3"/>
     </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B31" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="3"/>
-      <c r="D31" s="3">
+      <c r="D31" s="7">
         <v>1</v>
       </c>
       <c r="E31" s="3">
         <v>20</v>
       </c>
-      <c r="F31" s="3">
-        <v>100</v>
-      </c>
-      <c r="G31" s="3">
+      <c r="F31" s="7">
+        <v>100</v>
+      </c>
+      <c r="G31" s="7">
         <v>7</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="3" t="s">
+      <c r="K31" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L31" s="3"/>
-      <c r="M31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N31" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O31" s="3" t="s">
+      <c r="M31" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O31" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P31" s="3"/>
-      <c r="Q31" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R31" s="3" t="s">
+      <c r="Q31" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R31" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S31" s="3"/>
@@ -2089,44 +2252,44 @@
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C32" s="3"/>
-      <c r="D32" s="3">
+      <c r="D32" s="7">
         <v>1</v>
       </c>
       <c r="E32" s="3">
         <v>20</v>
       </c>
-      <c r="F32" s="3">
-        <v>100</v>
-      </c>
-      <c r="G32" s="3">
+      <c r="F32" s="7">
+        <v>100</v>
+      </c>
+      <c r="G32" s="7">
         <v>7</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
-      <c r="K32" s="3" t="s">
+      <c r="K32" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L32" s="3"/>
-      <c r="M32" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N32" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O32" s="3" t="s">
+      <c r="M32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N32" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O32" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P32" s="3"/>
-      <c r="Q32" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R32" s="3" t="s">
+      <c r="Q32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R32" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S32" s="3"/>
@@ -2134,44 +2297,44 @@
       <c r="U32" s="3"/>
       <c r="V32" s="3"/>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C33" s="3"/>
-      <c r="D33" s="3">
+      <c r="D33" s="7">
         <v>1</v>
       </c>
       <c r="E33" s="3">
         <v>20</v>
       </c>
-      <c r="F33" s="3">
-        <v>100</v>
-      </c>
-      <c r="G33" s="3">
+      <c r="F33" s="7">
+        <v>100</v>
+      </c>
+      <c r="G33" s="7">
         <v>7</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
-      <c r="K33" s="3" t="s">
+      <c r="K33" s="7" t="s">
         <v>22</v>
       </c>
       <c r="L33" s="3"/>
-      <c r="M33" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O33" s="3" t="s">
+      <c r="M33" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N33" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O33" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P33" s="3"/>
-      <c r="Q33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R33" s="3" t="s">
+      <c r="Q33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R33" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S33" s="3"/>
@@ -2179,7 +2342,7 @@
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -2202,7 +2365,7 @@
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
     </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -2223,7 +2386,7 @@
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
     </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2244,7 +2407,7 @@
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
     </row>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -2265,7 +2428,7 @@
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
     </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -2286,7 +2449,7 @@
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
     </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -2307,7 +2470,7 @@
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
     </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -2328,7 +2491,7 @@
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
     </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -2349,7 +2512,7 @@
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
     </row>
-    <row r="42" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -2370,7 +2533,7 @@
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
     </row>
-    <row r="43" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2391,7 +2554,7 @@
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
     </row>
-    <row r="44" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2412,7 +2575,7 @@
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
     </row>
-    <row r="45" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -2433,7 +2596,7 @@
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
     </row>
-    <row r="46" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -2454,7 +2617,7 @@
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
     </row>
-    <row r="47" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -2475,7 +2638,7 @@
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
     </row>
-    <row r="48" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -2496,7 +2659,7 @@
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
     </row>
-    <row r="49" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>

</xml_diff>